<commit_message>
add import Excel File
</commit_message>
<xml_diff>
--- a/storage/file.xlsx
+++ b/storage/file.xlsx
@@ -92,23 +92,23 @@
     <row r="2" spans="1:7">
       <c r="A2" s="0" t="inlineStr">
         <is>
-          <t>ناراحت</t>
+          <t>عاشق</t>
         </is>
       </c>
       <c r="B2" s="0">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" s="0">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D2" s="0" t="inlineStr">
         <is>
-          <t>2022-04-19 06:58:32</t>
+          <t>2022-04-17 11:36:00</t>
         </is>
       </c>
       <c r="E2" s="0" t="inlineStr">
         <is>
-          <t>سیک کن از سایت بیرون</t>
+          <t>اونایی که در خط امام نیستن</t>
         </is>
       </c>
       <c r="F2" s="0" t="inlineStr">
@@ -118,7 +118,7 @@
       </c>
       <c r="G2" s="0" t="inlineStr">
         <is>
-          <t>led</t>
+          <t>alireza</t>
         </is>
       </c>
     </row>
@@ -129,19 +129,19 @@
         </is>
       </c>
       <c r="B3" s="0">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3" s="0">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D3" s="0" t="inlineStr">
         <is>
-          <t>2022-04-17 11:35:49</t>
+          <t>2022-04-19 06:58:32</t>
         </is>
       </c>
       <c r="E3" s="0" t="inlineStr">
         <is>
-          <t>به شما ناهارمدادن ؟</t>
+          <t>سیک کن از سایت بیرون</t>
         </is>
       </c>
       <c r="F3" s="0" t="inlineStr">
@@ -162,29 +162,95 @@
         </is>
       </c>
       <c r="B4" s="0">
+        <v>3</v>
+      </c>
+      <c r="C4" s="0">
+        <v>12</v>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>2022-04-17 11:35:49</t>
+        </is>
+      </c>
+      <c r="E4" s="0" t="inlineStr">
+        <is>
+          <t>به شما ناهارمدادن ؟</t>
+        </is>
+      </c>
+      <c r="F4" s="0" t="inlineStr">
+        <is>
+          <t>Open</t>
+        </is>
+      </c>
+      <c r="G4" s="0" t="inlineStr">
+        <is>
+          <t>led</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="0" t="inlineStr">
+        <is>
+          <t>ناراحت</t>
+        </is>
+      </c>
+      <c r="B5" s="0">
         <v>4</v>
       </c>
-      <c r="C4" s="0">
+      <c r="C5" s="0">
         <v>3</v>
       </c>
-      <c r="D4" s="0" t="inlineStr">
+      <c r="D5" s="0" t="inlineStr">
         <is>
           <t>2022-04-19 10:38:55</t>
         </is>
       </c>
-      <c r="E4" s="0" t="inlineStr">
+      <c r="E5" s="0" t="inlineStr">
         <is>
           <t>جواب منو سریع بده</t>
         </is>
       </c>
-      <c r="F4" s="0" t="inlineStr">
+      <c r="F5" s="0" t="inlineStr">
         <is>
           <t>Customer-Reply</t>
         </is>
       </c>
-      <c r="G4" s="0" t="inlineStr">
+      <c r="G5" s="0" t="inlineStr">
         <is>
           <t>alireza</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="0" t="inlineStr">
+        <is>
+          <t>عاشق</t>
+        </is>
+      </c>
+      <c r="B6" s="0">
+        <v>5</v>
+      </c>
+      <c r="C6" s="0">
+        <v>10</v>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>2022-04-19 08:16:11</t>
+        </is>
+      </c>
+      <c r="E6" s="0" t="inlineStr">
+        <is>
+          <t>خرابی کد تخفیف</t>
+        </is>
+      </c>
+      <c r="F6" s="0" t="inlineStr">
+        <is>
+          <t>Answered</t>
+        </is>
+      </c>
+      <c r="G6" s="0" t="inlineStr">
+        <is>
+          <t>mamd</t>
         </is>
       </c>
     </row>

</xml_diff>